<commit_message>
sampai labeling manual, sesuai alur baru
</commit_message>
<xml_diff>
--- a/application/static/excel_data/data_crawling -- 1. #belajaronline.xlsx
+++ b/application/static/excel_data/data_crawling -- 1. #belajaronline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="284">
   <si>
     <t>id</t>
   </si>
@@ -1030,6 +1030,127 @@
   </si>
   <si>
     <t>Sat Dec 12 06:59:02 +0000 2020</t>
+  </si>
+  <si>
+    <t>Ini loh Mugwort yang lagi jadi holy grail-nya sobat tiktok sekalian karena emang hasilnya sebagus itu di muka :')
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #mugwort https://t.co/kArzlIgUUJ</t>
+  </si>
+  <si>
+    <t>Thu Dec 17 05:13:26 +0000 2020</t>
+  </si>
+  <si>
+    <t>Nilai aja yang tinggi nggak ada yang masuk di otak 
+#belajaronline</t>
+  </si>
+  <si>
+    <t>AbdSalam24</t>
+  </si>
+  <si>
+    <t>Thu Dec 17 01:39:54 +0000 2020</t>
+  </si>
+  <si>
+    <t>Yuk join ke Groupnya untuk informasi setiap minggunya di https://t.co/xjVIJXwfwr
+Bonjour Prancis
+One Third Consulting &amp;amp; Abroad
+#BonjourPrancis #lesbahasaprancis #konsultasipendidikan #belajaronline #beasiswa #beasiswaprancis #konsultasigratis #beasiswaeropa #bahasaprancis https://t.co/KZPrhCbrAs</t>
+  </si>
+  <si>
+    <t>BonjourPrancis</t>
+  </si>
+  <si>
+    <t>Wed Dec 16 05:40:02 +0000 2020</t>
+  </si>
+  <si>
+    <t>Ingat lagu ini? 
+.
+Sc twitter @tvindonesiawkwk
+.
+#kampuscenter #workshoplulusptn #PJJ #belajaronline #sma #kampus #pelajar #ltmpt #kuliah #UTBK #SBMPTN #snmptn2020  #ltmpt2020 #ltmpt #sbmptn2020 #utbk2020 #utbk #masukkampus #kampusindonesia https://t.co/v8g762UPK5</t>
+  </si>
+  <si>
+    <t>kampuscenter</t>
+  </si>
+  <si>
+    <t>Wed Dec 16 04:35:47 +0000 2020</t>
+  </si>
+  <si>
+    <t>Hari ini di kelas Jena kita membahas soal ujian minggu kemaren😁 Udah pada jago nih temen-temen, jangan lupa kudu PD ya buat sprechen nyaa👩‍💻👨‍💻
+#kursusbahasa #kursusonline #belajarjerman #belajaronline #ujian https://t.co/Wla9l8laOD</t>
+  </si>
+  <si>
+    <t>jermanstudiere</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 15:02:15 +0000 2020</t>
+  </si>
+  <si>
+    <t>Masih susah jamanku ya...
+.
+Sc: unknown (yang tau kasih tau bro)
+.
+.
+Reposted from @1cak
+.
+#workshoplulusptn #kampus #kampuscenter #belajaronline #sma #kampus #pelajar #ltmpt #kuliah #UTBK #SNMPTN #SBMPTN #snmptn2020  #ltmpt2020 #ltmpt #sbmptn2020 #utbk2020 #utbk #masukkampus https://t.co/HtJ87PPW5j</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 07:41:01 +0000 2020</t>
+  </si>
+  <si>
+    <t>Terima kasih, suhu~ @MelissaSunjaya 
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #tulisa https://t.co/gTFH9khSL7</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 05:42:19 +0000 2020</t>
+  </si>
+  <si>
+    <t>Ya, gimana ya. Aduh mba Mel, aku bingung menjelaskannya~
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #tulisa https://t.co/jYQwJNvBJr</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 05:41:31 +0000 2020</t>
+  </si>
+  <si>
+    <t>Iya plissss pulsa internet sama subscribe layanan streaming-nya sekalian~
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #tulisa https://t.co/d0b1vfWkvc</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 05:40:38 +0000 2020</t>
+  </si>
+  <si>
+    <t>Ga lengkap kalo ga lucu-lucuan, ya kan?!
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #tulisa https://t.co/vI793G1wc6</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 05:39:13 +0000 2020</t>
+  </si>
+  <si>
+    <t>Pas banget buat sobi twitter yang hobinya 2 a.m thoughts :")
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #tulisa https://t.co/nH1IVEfeHk</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 05:38:27 +0000 2020</t>
+  </si>
+  <si>
+    <t>Yang udah dapet jadwal tuker kado akhir tahun, sini dulu yuk!
+Ada rekomendasi kado paling 'sumpah ga ngerti lagi' dari Melissa Sunjaya biar momen tuker kado kamu lebih asik, lop.
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #tulisan https://t.co/od6zPaYitb</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 05:36:38 +0000 2020</t>
+  </si>
+  <si>
+    <t>Mau tahu cara praktis dan murah untuk Pembelajaran Jarak Jauh (PJJ)?👩‍💻
+Pasti mau kan... Saatnya kamu tinggalkan cara manual untuk mengatur jadwal kelas dan meeting secara virtual 📆.
+Solusinya, pakai https://t.co/1rIQ8ab0xT.
+#belajaronline 
+#fingerspot https://t.co/SlWG2pIvm4</t>
+  </si>
+  <si>
+    <t>Bambang90500845</t>
+  </si>
+  <si>
+    <t>Tue Dec 15 03:48:27 +0000 2020</t>
   </si>
 </sst>
 </file>
@@ -1394,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J121" sqref="J121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,6 +3063,216 @@
         <v>222</v>
       </c>
     </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1.3394385334260449E+18</v>
+      </c>
+      <c r="B111" t="s">
+        <v>253</v>
+      </c>
+      <c r="C111" t="s">
+        <v>17</v>
+      </c>
+      <c r="D111" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1.339384794988257E+18</v>
+      </c>
+      <c r="B112" t="s">
+        <v>255</v>
+      </c>
+      <c r="C112" t="s">
+        <v>256</v>
+      </c>
+      <c r="D112" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1.339082840617599E+18</v>
+      </c>
+      <c r="B113" t="s">
+        <v>258</v>
+      </c>
+      <c r="C113" t="s">
+        <v>259</v>
+      </c>
+      <c r="D113" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1.3390666690968251E+18</v>
+      </c>
+      <c r="B114" t="s">
+        <v>261</v>
+      </c>
+      <c r="C114" t="s">
+        <v>262</v>
+      </c>
+      <c r="D114" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1.3388619395862981E+18</v>
+      </c>
+      <c r="B115" t="s">
+        <v>264</v>
+      </c>
+      <c r="C115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D115" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1.338750899888374E+18</v>
+      </c>
+      <c r="B116" t="s">
+        <v>267</v>
+      </c>
+      <c r="C116" t="s">
+        <v>262</v>
+      </c>
+      <c r="D116" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1.338721025832362E+18</v>
+      </c>
+      <c r="B117" t="s">
+        <v>269</v>
+      </c>
+      <c r="C117" t="s">
+        <v>17</v>
+      </c>
+      <c r="D117" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1.338720825596236E+18</v>
+      </c>
+      <c r="B118" t="s">
+        <v>271</v>
+      </c>
+      <c r="C118" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1.3387206031891251E+18</v>
+      </c>
+      <c r="B119" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D119" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1.3387202467907169E+18</v>
+      </c>
+      <c r="B120" t="s">
+        <v>275</v>
+      </c>
+      <c r="C120" t="s">
+        <v>17</v>
+      </c>
+      <c r="D120" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1.338720054427337E+18</v>
+      </c>
+      <c r="B121" t="s">
+        <v>277</v>
+      </c>
+      <c r="C121" t="s">
+        <v>17</v>
+      </c>
+      <c r="D121" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1.3387195954236211E+18</v>
+      </c>
+      <c r="B122" t="s">
+        <v>279</v>
+      </c>
+      <c r="C122" t="s">
+        <v>17</v>
+      </c>
+      <c r="D122" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1.338692370167042E+18</v>
+      </c>
+      <c r="B123" t="s">
+        <v>281</v>
+      </c>
+      <c r="C123" t="s">
+        <v>282</v>
+      </c>
+      <c r="D123" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1.3384047881746061E+18</v>
+      </c>
+      <c r="B124" t="s">
+        <v>230</v>
+      </c>
+      <c r="C124" t="s">
+        <v>231</v>
+      </c>
+      <c r="D124" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1.338391443543532E+18</v>
+      </c>
+      <c r="B125" t="s">
+        <v>233</v>
+      </c>
+      <c r="C125" t="s">
+        <v>17</v>
+      </c>
+      <c r="D125" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add split data dan sampling kuota modelling
</commit_message>
<xml_diff>
--- a/application/static/excel_data/data_crawling -- 1. #belajaronline.xlsx
+++ b/application/static/excel_data/data_crawling -- 1. #belajaronline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="326">
   <si>
     <t>id</t>
   </si>
@@ -1243,6 +1243,73 @@
   </si>
   <si>
     <t>Fri Dec 18 05:18:04 +0000 2020</t>
+  </si>
+  <si>
+    <t>Yang lagi Headset Bass tapi murah spesial buat kamu 25ribu aja... Tidak bagus duit kembali full
+#original #newnormal #belajaronline #headset https://t.co/Kv3T05uz5v</t>
+  </si>
+  <si>
+    <t>Fri Dec 25 15:07:05 +0000 2020</t>
+  </si>
+  <si>
+    <t>Kamu bisa belajar hingga 14 sesi kelas online gratis di Kelas Pintar loh!
+#belajaronline #bimbinganbelajar #belajardirumah #bimbelterbaik #kelaspintarindonesia https://t.co/CP0jnmGbZw</t>
+  </si>
+  <si>
+    <t>kelaspintar_id</t>
+  </si>
+  <si>
+    <t>Fri Dec 25 09:01:41 +0000 2020</t>
+  </si>
+  <si>
+    <t>Selamat Hari Natal bagi semua yang merayakan!
+We wish you a wonderful christmast in every way🎄
+#Vyneapple #funlearning #keluarga #belajaronline #infoparenting #parenthood #parenting #parentingtips #edukasianak #merrychristmas #Christmas https://t.co/ys0Qsj7K5A</t>
+  </si>
+  <si>
+    <t>Fri Dec 25 04:33:56 +0000 2020</t>
+  </si>
+  <si>
+    <t>Selamat Hari Natal buat yang merayakan!
+Selamat tanggal merah buat yang liburan!
+Yok bahagia yok! Tahunnya bentar lagi ganti, nih.
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #SelamatHariNatal #MerryChristmas2020 https://t.co/AwAZ4Tjz5S</t>
+  </si>
+  <si>
+    <t>Fri Dec 25 03:00:02 +0000 2020</t>
+  </si>
+  <si>
+    <t>Di hari yang spesial ini, Kelaskita mau ngumumin siapa aja sih pemenang giveaway bingkisan cantik dari @mytulisan?
+Mampir ke Instagram @kelaskitadotcom, ya!
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja  #giveaway #tulisan https://t.co/vUKlKwY6xC</t>
+  </si>
+  <si>
+    <t>Tue Dec 22 08:13:41 +0000 2020</t>
+  </si>
+  <si>
+    <t>Rutinitas tiap hari
+#Belajaronline #pandemi #dirumahaja https://t.co/i4vf1xkGR8</t>
+  </si>
+  <si>
+    <t>itsnurmi</t>
+  </si>
+  <si>
+    <t>Tue Dec 22 06:20:10 +0000 2020</t>
+  </si>
+  <si>
+    <t>Yak abis ngucapin selamat hari Ibu, jangan lupa dibantu kerjaan Ibunya. Konteeeennn terosssss~
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #SelamatHariIbu</t>
+  </si>
+  <si>
+    <t>Tue Dec 22 03:09:33 +0000 2020</t>
+  </si>
+  <si>
+    <t>Selamat Hari Ibu, Bunda, Mama, Mami, Umi, Emak, dan semua Ibu yang sudah berjuang sekuat ini.
+Terima kasih cintaku sepanjang masa~
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #SelamatHariIbu https://t.co/4CQOub0r2j</t>
+  </si>
+  <si>
+    <t>Tue Dec 22 03:07:59 +0000 2020</t>
   </si>
 </sst>
 </file>
@@ -1607,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I139" sqref="I139"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3533,6 +3600,132 @@
         <v>257</v>
       </c>
     </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1.3424870312728451E+18</v>
+      </c>
+      <c r="B138" t="s">
+        <v>308</v>
+      </c>
+      <c r="C138" t="s">
+        <v>169</v>
+      </c>
+      <c r="D138" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1.342395076568363E+18</v>
+      </c>
+      <c r="B139" t="s">
+        <v>310</v>
+      </c>
+      <c r="C139" t="s">
+        <v>311</v>
+      </c>
+      <c r="D139" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>1.3423276943614159E+18</v>
+      </c>
+      <c r="B140" t="s">
+        <v>313</v>
+      </c>
+      <c r="C140" t="s">
+        <v>92</v>
+      </c>
+      <c r="D140" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>1.342304066517524E+18</v>
+      </c>
+      <c r="B141" t="s">
+        <v>315</v>
+      </c>
+      <c r="C141" t="s">
+        <v>17</v>
+      </c>
+      <c r="D141" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>1.3412958325076659E+18</v>
+      </c>
+      <c r="B142" t="s">
+        <v>317</v>
+      </c>
+      <c r="C142" t="s">
+        <v>17</v>
+      </c>
+      <c r="D142" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1.3412672677120251E+18</v>
+      </c>
+      <c r="B143" t="s">
+        <v>319</v>
+      </c>
+      <c r="C143" t="s">
+        <v>320</v>
+      </c>
+      <c r="D143" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1.3412192956158851E+18</v>
+      </c>
+      <c r="B144" t="s">
+        <v>322</v>
+      </c>
+      <c r="C144" t="s">
+        <v>17</v>
+      </c>
+      <c r="D144" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1.3412189007598589E+18</v>
+      </c>
+      <c r="B145" t="s">
+        <v>324</v>
+      </c>
+      <c r="C145" t="s">
+        <v>17</v>
+      </c>
+      <c r="D145" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1.340882051587744E+18</v>
+      </c>
+      <c r="B146" t="s">
+        <v>284</v>
+      </c>
+      <c r="C146" t="s">
+        <v>285</v>
+      </c>
+      <c r="D146" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add excel & jupyter
</commit_message>
<xml_diff>
--- a/application/static/excel_data/data_crawling -- 1. #belajaronline.xlsx
+++ b/application/static/excel_data/data_crawling -- 1. #belajaronline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="442">
   <si>
     <t>id</t>
   </si>
@@ -1631,6 +1631,139 @@
   </si>
   <si>
     <t>Thu Dec 31 06:28:55 +0000 2020</t>
+  </si>
+  <si>
+    <t>Tahun baru masih anget..5 Januari 2021. Persiapan Daring lg.
+#newyear
+#belajaronline
+#menantivaksin
+#covid19
+#bekasi</t>
+  </si>
+  <si>
+    <t>dannyurban</t>
+  </si>
+  <si>
+    <t>Tue Jan 05 10:16:10 +0000 2021</t>
+  </si>
+  <si>
+    <t>Last but not least, asik!
+Terus perluas jaringan dan kenal sama orang baru biar tau kisah-kisah keberhasilan mereka. Et, tapi tetap harus optimis juga sama diri sendiri.
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja https://t.co/t9tDGJLoCe</t>
+  </si>
+  <si>
+    <t>Tue Jan 05 05:04:22 +0000 2021</t>
+  </si>
+  <si>
+    <t>Emang butuh pede yang besar buat ngubah sesuatu dan belajar hal baru, tapi ya harus pede! 
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja https://t.co/55WbqzVRLF</t>
+  </si>
+  <si>
+    <t>Tue Jan 05 05:00:35 +0000 2021</t>
+  </si>
+  <si>
+    <t>Harus berani cari tantangan baru, ya namanya juga keluar zona nyaman~
+Evaluasi juga jangan ditinggalin.
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja https://t.co/8O6hMK65QF</t>
+  </si>
+  <si>
+    <t>Tue Jan 05 04:59:13 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mau ngumpulin orang-orang yang lagi bangun niat buat keluar dari zona nyaman, nih!
+Simak tipsnya yuk!
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja https://t.co/FZfGa6PoVy</t>
+  </si>
+  <si>
+    <t>Tue Jan 05 04:58:11 +0000 2021</t>
+  </si>
+  <si>
+    <t>Promo layar Interaktif Flat Panel ukuran layar lebar 65 inch ... Hub. 081386785850 @mandiriartha #korporasijabar #mandiriarthasolusi  #interaktifflatpanel #pembelajaranjarakjauh #belajaronline #bekerjajarakjauh #wfh https://t.co/rUQ11W3LWv</t>
+  </si>
+  <si>
+    <t>echo_kilo_oscar</t>
+  </si>
+  <si>
+    <t>Tue Jan 05 00:12:38 +0000 2021</t>
+  </si>
+  <si>
+    <t>Pergulatan peronlinenan ummat dimulai..
+kau membentukku semakin tangguh..
+semangat berproses kembali dan semoga cerita yang kita gores lebih berwarna nan bermakna..
+#seninvibbes #postivvibes #semangatsenin #belajaronline #dirumahsaja https://t.co/mUQ8gsnUDC</t>
+  </si>
+  <si>
+    <t>sofi_ksmnrsh</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 16:03:00 +0000 2021</t>
+  </si>
+  <si>
+    <t>Pemerintah pusat mengizinkan pemerintah daerah untuk melaksanakan pembelajaran tatap muka (PTM).
+#BelajarDariRumah #belajaronline #daring #KBM #UPI #IKAUPI #lampung #lampostco
+https://t.co/rb8U9YjcY0</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 13:37:35 +0000 2021</t>
+  </si>
+  <si>
+    <t>Halo sobat Homelab
+Jadikan kegagalan itu sebuah bukti kamu pernah berjuang dan jangan berhenti disituasi itu tapi selesaikan perjuanganmu sampai tuntas dan berhasil!
+#homelab #askhomelab #belajarbarengberkolaborasibareng #belajardimanasaja #elearning #belajaronline https://t.co/4LT3plS06D</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 12:13:00 +0000 2021</t>
+  </si>
+  <si>
+    <t>Dinas Pendidikan Kabupaten Pesawaran, memutuskan kegiatan belajar mengajar (KBM) tatap muka di Bumi Andan Jejama diundur sampai waktu yang belum ditentukan.
+#BelajarDariRumah #belajaronline #daring #KBM #pesawaran #lampung #lampostco
+https://t.co/SQduyCyQxr</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 10:36:31 +0000 2021</t>
+  </si>
+  <si>
+    <t>Makan sekuteng di rawa-rawa
+Kelaskita dateng bawa kabar gembira!
+Akhirnya pantun go Internasional, gais!
+#kelaskita #carabarubelajarseru #belajardirumah #elearning #belajaronline #dirumahaja #taugaksih https://t.co/cJ6ld6Yok4</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 07:00:12 +0000 2021</t>
+  </si>
+  <si>
+    <t>Hi Fellas! Tak perlu repot-repot pergi ke lembaga kursus, Lister siap membantu Kamu jadi lebih hebat di tahun 2021. 
+#belajaronline #lister #kursusielts #kursustoelf #kursusbahasaasing #kursusbimbinganbeasiswa #listerlanguagemaster https://t.co/QeToE9CDb4</t>
+  </si>
+  <si>
+    <t>lister_id</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 04:57:41 +0000 2021</t>
+  </si>
+  <si>
+    <t>Kion Kids mengandung Ion Negatif &amp;amp; FIR yang bantu jaga kesehatan mata siBuah Hati.
+#kionnanokids
+#kacamatakesehatan
+#belajaronline
+#inspiradzi
+#digitalnetworkmarketing</t>
+  </si>
+  <si>
+    <t>SusantoSane</t>
+  </si>
+  <si>
+    <t>Mon Jan 04 01:44:07 +0000 2021</t>
+  </si>
+  <si>
+    <t>Jadwal Baru Belajar dari Rumah TVRI untuk PAUD dan SD Kelas 1-6, Tiap Senin-Jumat Selama 30 Menit
+https://t.co/kk7OLxdr7G #JadwalBaru #BelajarDariRumah #TVRI #BelajarOnline</t>
+  </si>
+  <si>
+    <t>tribunkaltim</t>
+  </si>
+  <si>
+    <t>Sat Jan 02 22:26:41 +0000 2021</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K177" sqref="K177"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J206" sqref="J206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4761,6 +4894,230 @@
         <v>356</v>
       </c>
     </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>1.3464000889695439E+18</v>
+      </c>
+      <c r="B198" t="s">
+        <v>408</v>
+      </c>
+      <c r="C198" t="s">
+        <v>409</v>
+      </c>
+      <c r="D198" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>1.3463216211418729E+18</v>
+      </c>
+      <c r="B199" t="s">
+        <v>411</v>
+      </c>
+      <c r="C199" t="s">
+        <v>17</v>
+      </c>
+      <c r="D199" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>1.3463206669207959E+18</v>
+      </c>
+      <c r="B200" t="s">
+        <v>413</v>
+      </c>
+      <c r="C200" t="s">
+        <v>17</v>
+      </c>
+      <c r="D200" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>1.3463203249172969E+18</v>
+      </c>
+      <c r="B201" t="s">
+        <v>415</v>
+      </c>
+      <c r="C201" t="s">
+        <v>17</v>
+      </c>
+      <c r="D201" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>1.3463200637170161E+18</v>
+      </c>
+      <c r="B202" t="s">
+        <v>417</v>
+      </c>
+      <c r="C202" t="s">
+        <v>17</v>
+      </c>
+      <c r="D202" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>1.3462482020396401E+18</v>
+      </c>
+      <c r="B203" t="s">
+        <v>419</v>
+      </c>
+      <c r="C203" t="s">
+        <v>420</v>
+      </c>
+      <c r="D203" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>1.3461249850525E+18</v>
+      </c>
+      <c r="B204" t="s">
+        <v>422</v>
+      </c>
+      <c r="C204" t="s">
+        <v>423</v>
+      </c>
+      <c r="D204" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>1.3460883879381399E+18</v>
+      </c>
+      <c r="B205" t="s">
+        <v>425</v>
+      </c>
+      <c r="C205" t="s">
+        <v>380</v>
+      </c>
+      <c r="D205" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>1.346067103321739E+18</v>
+      </c>
+      <c r="B206" t="s">
+        <v>427</v>
+      </c>
+      <c r="C206" t="s">
+        <v>327</v>
+      </c>
+      <c r="D206" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>1.346042820201599E+18</v>
+      </c>
+      <c r="B207" t="s">
+        <v>429</v>
+      </c>
+      <c r="C207" t="s">
+        <v>380</v>
+      </c>
+      <c r="D207" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>1.345988381856076E+18</v>
+      </c>
+      <c r="B208" t="s">
+        <v>431</v>
+      </c>
+      <c r="C208" t="s">
+        <v>17</v>
+      </c>
+      <c r="D208" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>1.345957551767126E+18</v>
+      </c>
+      <c r="B209" t="s">
+        <v>433</v>
+      </c>
+      <c r="C209" t="s">
+        <v>434</v>
+      </c>
+      <c r="D209" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>1.345908839414071E+18</v>
+      </c>
+      <c r="B210" t="s">
+        <v>436</v>
+      </c>
+      <c r="C210" t="s">
+        <v>437</v>
+      </c>
+      <c r="D210" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>1.3454967659364559E+18</v>
+      </c>
+      <c r="B211" t="s">
+        <v>439</v>
+      </c>
+      <c r="C211" t="s">
+        <v>440</v>
+      </c>
+      <c r="D211" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>1.345339053508415E+18</v>
+      </c>
+      <c r="B212" t="s">
+        <v>386</v>
+      </c>
+      <c r="C212" t="s">
+        <v>387</v>
+      </c>
+      <c r="D212" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>1.345216933696705E+18</v>
+      </c>
+      <c r="B213" t="s">
+        <v>389</v>
+      </c>
+      <c r="C213" t="s">
+        <v>390</v>
+      </c>
+      <c r="D213" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>